<commit_message>
titles work with styling
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -19,19 +19,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>row_header_1</t>
   </si>
   <si>
     <t>column_header_1</t>
   </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>spacer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,8 +78,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,8 +106,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,17 +132,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -448,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -459,14 +506,44 @@
     <col min="1" max="1" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" ht="32" customHeight="1">
+    <row r="3" spans="1:2" ht="32" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added autodetect row format and combine columns
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>row_header_1</t>
   </si>
@@ -34,13 +34,28 @@
   </si>
   <si>
     <t>spacer</t>
+  </si>
+  <si>
+    <t>indent_1</t>
+  </si>
+  <si>
+    <t>indent_2</t>
+  </si>
+  <si>
+    <t>indent_3</t>
+  </si>
+  <si>
+    <t>indent_4</t>
+  </si>
+  <si>
+    <t>indent_5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,8 +107,32 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +148,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -147,7 +216,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -162,6 +231,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -495,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -546,6 +620,46 @@
         <v>20</v>
       </c>
     </row>
+    <row r="11" spans="1:2" ht="18">
+      <c r="A11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
row styles now work
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>row_header_1</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>indent_5</t>
+  </si>
+  <si>
+    <t>indent_0</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +181,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,12 +220,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -236,10 +249,15 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -620,44 +638,52 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:2" ht="20">
+      <c r="A11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18">
+      <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B11">
+      <c r="B13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13">
+    <row r="17" spans="1:2">
+      <c r="A17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15">
+    <row r="19" spans="1:2">
+      <c r="A19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17">
+    <row r="21" spans="1:2">
+      <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="10" t="s">
+      <c r="B21">
         <v>9</v>
-      </c>
-      <c r="B19">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enabled style overrides and autodetect column style
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,12 +156,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -187,6 +181,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,12 +244,22 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -590,7 +600,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -639,7 +649,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="20">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -647,7 +657,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="18">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B13">
@@ -655,7 +665,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B15">
@@ -663,7 +673,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B17">
@@ -671,7 +681,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B19">
@@ -679,7 +689,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B21">

</xml_diff>

<commit_message>
almost there currently adding fix for colours returning as theme numbers
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>row_header_1</t>
   </si>
@@ -52,13 +52,16 @@
   </si>
   <si>
     <t>indent_0</t>
+  </si>
+  <si>
+    <t>body</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,6 +134,19 @@
     <font>
       <sz val="6"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="2"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -229,7 +245,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -244,7 +260,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -260,6 +275,8 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -597,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -649,7 +666,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="20">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -657,7 +674,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="18">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B13">
@@ -665,7 +682,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B15">
@@ -673,7 +690,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B17">
@@ -681,7 +698,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B19">
@@ -689,11 +706,19 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B21">
         <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some problems with styles.xlsx
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -288,19 +288,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -652,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -758,7 +750,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="18">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B25">
@@ -766,7 +758,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B27">
@@ -774,7 +766,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B29">
@@ -782,7 +774,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B31">
@@ -790,7 +782,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B33">
@@ -798,7 +790,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B35">

</xml_diff>

<commit_message>
fix bugs with indents and styles
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>row_header_1</t>
-  </si>
-  <si>
-    <t>column_header_1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>title</t>
   </si>
@@ -76,13 +70,16 @@
   </si>
   <si>
     <t>footer</t>
+  </si>
+  <si>
+    <t>top_header_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,12 +112,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -167,18 +158,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -267,22 +252,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -299,11 +281,11 @@
       <alignment horizontal="left" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -653,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -666,153 +648,145 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="32" customHeight="1">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" ht="28" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="28" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="B5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="4" t="s">
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="27" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
       <c r="B11">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:2" ht="18">
+      <c r="A23" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B23">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="18">
-      <c r="A25" s="13" t="s">
-        <v>12</v>
-      </c>
       <c r="B25">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
         <v>13</v>
       </c>
-      <c r="B27">
-        <v>15</v>
-      </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="15" t="s">
-        <v>14</v>
+      <c r="A29" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="B29">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B31">
+      <c r="B33">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="16" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B33">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="B35">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed left headers when autoindent
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,27 +132,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="9"/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -252,7 +259,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -264,7 +271,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -281,11 +287,13 @@
       <alignment horizontal="left" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -638,7 +646,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -687,7 +695,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B11">
@@ -695,7 +703,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B13">
@@ -703,7 +711,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B15">
@@ -711,7 +719,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B17">
@@ -719,7 +727,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B19">
@@ -727,31 +735,31 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B21">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18">
-      <c r="A23" s="12" t="s">
+    <row r="23" spans="1:2" ht="20">
+      <c r="A23" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B23">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="13" t="s">
+    <row r="25" spans="1:2" ht="18">
+      <c r="A25" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B25">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:2" ht="16">
+      <c r="A27" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B27">
@@ -759,7 +767,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B29">
@@ -767,7 +775,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B31">
@@ -775,7 +783,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B33">
@@ -783,7 +791,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B35">

</xml_diff>

<commit_message>
updated to make indent names more flexible
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="10780" yWindow="1680" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,12 +126,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="9"/>
       <color theme="1"/>
@@ -146,26 +140,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +198,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,13 +286,13 @@
       <alignment horizontal="left" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -646,7 +645,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -743,7 +742,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="20">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B23">
@@ -751,7 +750,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="18">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B25">
@@ -759,7 +758,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="16">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B27">

</xml_diff>

<commit_message>
added user ability to supply their own styles and num styles csv
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>title</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>top_header_1</t>
+  </si>
+  <si>
+    <t>right_border</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -236,6 +239,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -258,7 +270,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -293,6 +305,7 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -642,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -797,6 +810,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
moved simdata so tests don't error
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -115,13 +115,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="8"/>
       <color theme="1"/>
@@ -157,6 +150,13 @@
     <font>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -276,11 +276,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -298,14 +295,17 @@
       <alignment horizontal="left" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -675,7 +675,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="28" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B3">
@@ -707,7 +707,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B11">
@@ -715,7 +715,7 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B13">
@@ -723,7 +723,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B15">
@@ -731,7 +731,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B17">
@@ -739,7 +739,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B19">
@@ -747,7 +747,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B21">
@@ -755,7 +755,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="20">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B23">
@@ -763,7 +763,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="18">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B25">
@@ -771,7 +771,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="16">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B27">
@@ -779,7 +779,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B29">
@@ -787,7 +787,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B31">
@@ -795,7 +795,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B33">
@@ -803,7 +803,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B35">
@@ -811,7 +811,7 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B37">

</xml_diff>

<commit_message>
added borders to default styles and updated screenshots
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="1680" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3780" yWindow="2020" windowWidth="32600" windowHeight="15720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -220,20 +220,29 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color theme="1" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -280,20 +289,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -646,7 +655,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -655,7 +664,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B1">
@@ -663,7 +672,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="28" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B3">
@@ -671,7 +680,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B5">
@@ -743,7 +752,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="20">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B23">
@@ -751,7 +760,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="18">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B25">
@@ -759,7 +768,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="16">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B27">
@@ -767,7 +776,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B29">
@@ -775,7 +784,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B31">
@@ -799,7 +808,7 @@
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B37">

</xml_diff>

<commit_message>
got rid of row heights from test spreadsheets
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -652,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:A37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -663,156 +663,99 @@
     <col min="1" max="1" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="28" customHeight="1">
+    </row>
+    <row r="3" spans="1:1" ht="28" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="27" customHeight="1">
+    </row>
+    <row r="7" spans="1:1" ht="27" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+    </row>
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+    </row>
+    <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B11">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+    </row>
+    <row r="13" spans="1:1">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B13">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+    </row>
+    <row r="15" spans="1:1">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B17">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+    </row>
+    <row r="21" spans="1:1">
       <c r="A21" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B21">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="20">
+    </row>
+    <row r="23" spans="1:1" ht="20">
       <c r="A23" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B23">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="18">
+    </row>
+    <row r="25" spans="1:1" ht="18">
       <c r="A25" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B25">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="16">
+    </row>
+    <row r="27" spans="1:1" ht="16">
       <c r="A27" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B27">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+    </row>
+    <row r="29" spans="1:1">
       <c r="A29" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B29">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+    </row>
+    <row r="31" spans="1:1">
       <c r="A31" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B31">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+    </row>
+    <row r="33" spans="1:1">
       <c r="A33" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B33">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+    </row>
+    <row r="35" spans="1:1">
       <c r="A35" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B35">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+    </row>
+    <row r="37" spans="1:1">
       <c r="A37" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="B37">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enabled customisation of auto tab
</commit_message>
<xml_diff>
--- a/inst/extdata/styles.xlsx
+++ b/inst/extdata/styles.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>title</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>right_border</t>
+  </si>
+  <si>
+    <t>heavy_bottom_border</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -245,6 +248,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -267,7 +279,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -303,6 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -652,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -758,6 +771,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="39" spans="1:1" ht="16" thickBot="1">
+      <c r="A39" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>